<commit_message>
[MS-OXCMAPIHTTP] workitem 711961:[MS-OXCMAPIHTTP] Add new test cases for 37 requirements for 9 fixed TDIs
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -10034,9 +10034,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -11610,7 +11608,7 @@
         <v>15</v>
       </c>
       <c r="H69" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I69" s="31"/>
     </row>
@@ -11660,7 +11658,7 @@
         <v>15</v>
       </c>
       <c r="H71" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I71" s="31"/>
     </row>
@@ -12214,7 +12212,7 @@
         <v>15</v>
       </c>
       <c r="H93" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I93" s="31"/>
     </row>
@@ -12314,7 +12312,7 @@
         <v>15</v>
       </c>
       <c r="H97" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I97" s="31"/>
     </row>
@@ -12339,7 +12337,7 @@
         <v>15</v>
       </c>
       <c r="H98" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I98" s="31"/>
     </row>
@@ -12820,13 +12818,13 @@
         <v>19</v>
       </c>
       <c r="F117" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G117" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H117" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I117" s="31"/>
     </row>
@@ -12876,7 +12874,7 @@
         <v>15</v>
       </c>
       <c r="H119" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I119" s="31"/>
     </row>
@@ -12931,7 +12929,7 @@
       <c r="I121" s="31"/>
     </row>
     <row r="122" spans="1:9" ht="30">
-      <c r="A122" s="29" t="s">
+      <c r="A122" s="22" t="s">
         <v>107</v>
       </c>
       <c r="B122" s="30" t="s">
@@ -13095,7 +13093,7 @@
         <v>19</v>
       </c>
       <c r="F128" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G128" s="29" t="s">
         <v>15</v>
@@ -13120,7 +13118,7 @@
         <v>19</v>
       </c>
       <c r="F129" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G129" s="29" t="s">
         <v>15</v>
@@ -13145,7 +13143,7 @@
         <v>19</v>
       </c>
       <c r="F130" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G130" s="29" t="s">
         <v>15</v>
@@ -13170,7 +13168,7 @@
         <v>19</v>
       </c>
       <c r="F131" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G131" s="29" t="s">
         <v>16</v>
@@ -15011,7 +15009,7 @@
         <v>15</v>
       </c>
       <c r="H202" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I202" s="31"/>
     </row>
@@ -15036,7 +15034,7 @@
         <v>15</v>
       </c>
       <c r="H203" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I203" s="31"/>
     </row>
@@ -16863,7 +16861,7 @@
         <v>15</v>
       </c>
       <c r="H276" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I276" s="31"/>
     </row>
@@ -16888,7 +16886,7 @@
         <v>15</v>
       </c>
       <c r="H277" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I277" s="31"/>
     </row>
@@ -16913,7 +16911,7 @@
         <v>15</v>
       </c>
       <c r="H278" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I278" s="31"/>
     </row>
@@ -16963,7 +16961,7 @@
         <v>15</v>
       </c>
       <c r="H280" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I280" s="31"/>
     </row>
@@ -16988,7 +16986,7 @@
         <v>15</v>
       </c>
       <c r="H281" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I281" s="31"/>
     </row>
@@ -18015,7 +18013,7 @@
         <v>15</v>
       </c>
       <c r="H322" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I322" s="31"/>
     </row>
@@ -18040,7 +18038,7 @@
         <v>15</v>
       </c>
       <c r="H323" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I323" s="31"/>
     </row>
@@ -18065,7 +18063,7 @@
         <v>15</v>
       </c>
       <c r="H324" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I324" s="31"/>
     </row>
@@ -18115,7 +18113,7 @@
         <v>15</v>
       </c>
       <c r="H326" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I326" s="31"/>
     </row>
@@ -18140,7 +18138,7 @@
         <v>15</v>
       </c>
       <c r="H327" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I327" s="31"/>
     </row>
@@ -18592,7 +18590,7 @@
         <v>15</v>
       </c>
       <c r="H345" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I345" s="31"/>
     </row>
@@ -18617,7 +18615,7 @@
         <v>15</v>
       </c>
       <c r="H346" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I346" s="31"/>
     </row>
@@ -18642,7 +18640,7 @@
         <v>15</v>
       </c>
       <c r="H347" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I347" s="31"/>
     </row>
@@ -18667,7 +18665,7 @@
         <v>15</v>
       </c>
       <c r="H348" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I348" s="31"/>
     </row>
@@ -18692,7 +18690,7 @@
         <v>15</v>
       </c>
       <c r="H349" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I349" s="31"/>
     </row>
@@ -19419,7 +19417,7 @@
         <v>15</v>
       </c>
       <c r="H378" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I378" s="31"/>
     </row>
@@ -19444,7 +19442,7 @@
         <v>15</v>
       </c>
       <c r="H379" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I379" s="31"/>
     </row>
@@ -19469,7 +19467,7 @@
         <v>15</v>
       </c>
       <c r="H380" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I380" s="31"/>
     </row>
@@ -19494,7 +19492,7 @@
         <v>15</v>
       </c>
       <c r="H381" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I381" s="31"/>
     </row>
@@ -19519,7 +19517,7 @@
         <v>15</v>
       </c>
       <c r="H382" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I382" s="31"/>
     </row>
@@ -40976,7 +40974,7 @@
         <v>15</v>
       </c>
       <c r="H1237" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1237" s="31"/>
     </row>
@@ -41380,7 +41378,7 @@
         <v>15</v>
       </c>
       <c r="H1253" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1253" s="31"/>
     </row>
@@ -42005,7 +42003,7 @@
         <v>15</v>
       </c>
       <c r="H1278" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1278" s="31"/>
     </row>
@@ -42105,7 +42103,7 @@
         <v>15</v>
       </c>
       <c r="H1282" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1282" s="31"/>
     </row>
@@ -42180,7 +42178,7 @@
         <v>15</v>
       </c>
       <c r="H1285" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1285" s="31"/>
     </row>
@@ -42305,7 +42303,7 @@
         <v>15</v>
       </c>
       <c r="H1290" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1290" s="31"/>
     </row>

</xml_diff>

<commit_message>
[MS-OXCMAPIHTTP] workitem 711961: Add new test cases for 37 requirements for 9 fixed TDIs
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -9108,21 +9108,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9146,6 +9131,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10088,127 +10088,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10221,12 +10221,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10239,12 +10239,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10257,12 +10257,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10275,60 +10275,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -41403,7 +41403,7 @@
         <v>15</v>
       </c>
       <c r="H1254" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1254" s="31"/>
     </row>
@@ -42278,7 +42278,7 @@
         <v>15</v>
       </c>
       <c r="H1289" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1289" s="31"/>
     </row>
@@ -42900,6 +42900,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42907,11 +42912,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I124 A1306:I1313 A1305:H1305 A20:H1302 A69:I1304">

</xml_diff>

<commit_message>
[MS-OXCMAPIHTTP] fix workitem 711957: Add new 4+ test case for X-DeviceInfo Header field and  X-ClientInfo Header Field
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -9108,21 +9108,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9146,6 +9131,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10088,127 +10088,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10221,12 +10221,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10239,12 +10239,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10257,12 +10257,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10275,60 +10275,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -14853,13 +14853,13 @@
         <v>19</v>
       </c>
       <c r="F196" s="22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G196" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H196" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I196" s="31"/>
     </row>
@@ -14878,13 +14878,13 @@
         <v>19</v>
       </c>
       <c r="F197" s="22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G197" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H197" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I197" s="31"/>
     </row>
@@ -15409,7 +15409,7 @@
         <v>15</v>
       </c>
       <c r="H218" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I218" s="31"/>
     </row>
@@ -15434,7 +15434,7 @@
         <v>15</v>
       </c>
       <c r="H219" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I219" s="31"/>
     </row>
@@ -15534,7 +15534,7 @@
         <v>15</v>
       </c>
       <c r="H223" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I223" s="31"/>
     </row>
@@ -15584,7 +15584,7 @@
         <v>15</v>
       </c>
       <c r="H225" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I225" s="31"/>
     </row>
@@ -15634,7 +15634,7 @@
         <v>15</v>
       </c>
       <c r="H227" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I227" s="31"/>
     </row>
@@ -42900,6 +42900,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42907,11 +42912,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I124 A1306:I1313 A1305:H1305 A20:H1302 A69:I1304">

</xml_diff>

<commit_message>
[MS-OXCMAPIHTTP] Add new 10+ test cases for AddressBookPropertyValue, AddressBookTaggedPropertyValue,AddressBookTypedPropertyValue, AddressBookFlaggedPropertyValue and AddressBookFlaggedPropertyValueWithType.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -9108,6 +9108,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9131,21 +9146,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10088,127 +10088,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10221,12 +10221,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10239,12 +10239,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10257,12 +10257,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10275,60 +10275,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -10708,7 +10708,7 @@
         <v>15</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I33" s="24"/>
     </row>
@@ -10983,7 +10983,7 @@
         <v>15</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I44" s="24"/>
     </row>
@@ -11008,7 +11008,7 @@
         <v>15</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I45" s="24"/>
     </row>
@@ -11033,7 +11033,7 @@
         <v>15</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I46" s="24"/>
     </row>
@@ -11133,7 +11133,7 @@
         <v>15</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I50" s="24"/>
     </row>
@@ -11183,7 +11183,7 @@
         <v>15</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I52" s="24"/>
     </row>
@@ -11558,7 +11558,7 @@
         <v>15</v>
       </c>
       <c r="H67" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I67" s="24"/>
     </row>
@@ -42900,11 +42900,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42912,6 +42907,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I124 A1306:I1313 A1305:H1305 A20:H1302 A69:I1304">

</xml_diff>

<commit_message>
[MS-OXCMAPIHTTP]: Add failure response structure of Address Book Request Types
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -9108,6 +9108,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9131,21 +9146,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10034,13 +10034,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
@@ -10090,127 +10088,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10223,12 +10221,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10241,12 +10239,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10259,12 +10257,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10277,60 +10275,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -20325,7 +20323,7 @@
         <v>15</v>
       </c>
       <c r="H414" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I414" s="31"/>
     </row>
@@ -20350,7 +20348,7 @@
         <v>15</v>
       </c>
       <c r="H415" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I415" s="31"/>
     </row>
@@ -20375,7 +20373,7 @@
         <v>15</v>
       </c>
       <c r="H416" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I416" s="31"/>
     </row>
@@ -20400,7 +20398,7 @@
         <v>15</v>
       </c>
       <c r="H417" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I417" s="31"/>
     </row>
@@ -20425,7 +20423,7 @@
         <v>15</v>
       </c>
       <c r="H418" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I418" s="31"/>
     </row>
@@ -21002,7 +21000,7 @@
         <v>15</v>
       </c>
       <c r="H441" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I441" s="31"/>
     </row>
@@ -21027,7 +21025,7 @@
         <v>15</v>
       </c>
       <c r="H442" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I442" s="31"/>
     </row>
@@ -21052,7 +21050,7 @@
         <v>15</v>
       </c>
       <c r="H443" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I443" s="31"/>
     </row>
@@ -21102,7 +21100,7 @@
         <v>15</v>
       </c>
       <c r="H445" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I445" s="31"/>
     </row>
@@ -21127,7 +21125,7 @@
         <v>15</v>
       </c>
       <c r="H446" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I446" s="31"/>
     </row>
@@ -21152,7 +21150,7 @@
         <v>15</v>
       </c>
       <c r="H447" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I447" s="31"/>
     </row>
@@ -21979,7 +21977,7 @@
         <v>15</v>
       </c>
       <c r="H480" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I480" s="31"/>
     </row>
@@ -22004,7 +22002,7 @@
         <v>15</v>
       </c>
       <c r="H481" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I481" s="31"/>
     </row>
@@ -22029,7 +22027,7 @@
         <v>15</v>
       </c>
       <c r="H482" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I482" s="31"/>
     </row>
@@ -22054,7 +22052,7 @@
         <v>15</v>
       </c>
       <c r="H483" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I483" s="31"/>
     </row>
@@ -22079,7 +22077,7 @@
         <v>15</v>
       </c>
       <c r="H484" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I484" s="31"/>
     </row>
@@ -22906,7 +22904,7 @@
         <v>15</v>
       </c>
       <c r="H517" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I517" s="31"/>
     </row>
@@ -22931,7 +22929,7 @@
         <v>15</v>
       </c>
       <c r="H518" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I518" s="31"/>
     </row>
@@ -22956,7 +22954,7 @@
         <v>15</v>
       </c>
       <c r="H519" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I519" s="31"/>
     </row>
@@ -22981,7 +22979,7 @@
         <v>15</v>
       </c>
       <c r="H520" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I520" s="31"/>
     </row>
@@ -23006,7 +23004,7 @@
         <v>15</v>
       </c>
       <c r="H521" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I521" s="31"/>
     </row>
@@ -24733,7 +24731,7 @@
         <v>15</v>
       </c>
       <c r="H590" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I590" s="31"/>
     </row>
@@ -24758,7 +24756,7 @@
         <v>15</v>
       </c>
       <c r="H591" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I591" s="31"/>
     </row>
@@ -24783,7 +24781,7 @@
         <v>15</v>
       </c>
       <c r="H592" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I592" s="31"/>
     </row>
@@ -24808,7 +24806,7 @@
         <v>15</v>
       </c>
       <c r="H593" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I593" s="31"/>
     </row>
@@ -24833,7 +24831,7 @@
         <v>15</v>
       </c>
       <c r="H594" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I594" s="31"/>
     </row>
@@ -25489,7 +25487,7 @@
         <v>15</v>
       </c>
       <c r="H620" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I620" s="31"/>
     </row>
@@ -25514,7 +25512,7 @@
         <v>15</v>
       </c>
       <c r="H621" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I621" s="31"/>
     </row>
@@ -25539,7 +25537,7 @@
         <v>15</v>
       </c>
       <c r="H622" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I622" s="31"/>
     </row>
@@ -25564,7 +25562,7 @@
         <v>15</v>
       </c>
       <c r="H623" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I623" s="31"/>
     </row>
@@ -25589,7 +25587,7 @@
         <v>15</v>
       </c>
       <c r="H624" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I624" s="31"/>
     </row>
@@ -26372,7 +26370,7 @@
         <v>15</v>
       </c>
       <c r="H655" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I655" s="31"/>
     </row>
@@ -26397,7 +26395,7 @@
         <v>15</v>
       </c>
       <c r="H656" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I656" s="31"/>
     </row>
@@ -26422,7 +26420,7 @@
         <v>15</v>
       </c>
       <c r="H657" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I657" s="31"/>
     </row>
@@ -26447,7 +26445,7 @@
         <v>15</v>
       </c>
       <c r="H658" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I658" s="31"/>
     </row>
@@ -26472,7 +26470,7 @@
         <v>15</v>
       </c>
       <c r="H659" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I659" s="31"/>
     </row>
@@ -27453,7 +27451,7 @@
         <v>15</v>
       </c>
       <c r="H698" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I698" s="31"/>
     </row>
@@ -27478,7 +27476,7 @@
         <v>15</v>
       </c>
       <c r="H699" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I699" s="31"/>
     </row>
@@ -27503,7 +27501,7 @@
         <v>15</v>
       </c>
       <c r="H700" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I700" s="31"/>
     </row>
@@ -27528,7 +27526,7 @@
         <v>15</v>
       </c>
       <c r="H701" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I701" s="31"/>
     </row>
@@ -27553,7 +27551,7 @@
         <v>15</v>
       </c>
       <c r="H702" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I702" s="31"/>
     </row>
@@ -28359,7 +28357,7 @@
         <v>15</v>
       </c>
       <c r="H734" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I734" s="31"/>
     </row>
@@ -28384,7 +28382,7 @@
         <v>15</v>
       </c>
       <c r="H735" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I735" s="31"/>
     </row>
@@ -28409,7 +28407,7 @@
         <v>15</v>
       </c>
       <c r="H736" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I736" s="31"/>
     </row>
@@ -28434,7 +28432,7 @@
         <v>15</v>
       </c>
       <c r="H737" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I737" s="31"/>
     </row>
@@ -28459,7 +28457,7 @@
         <v>15</v>
       </c>
       <c r="H738" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I738" s="31"/>
     </row>
@@ -29323,7 +29321,7 @@
         <v>15</v>
       </c>
       <c r="H772" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I772" s="31"/>
     </row>
@@ -29348,7 +29346,7 @@
         <v>15</v>
       </c>
       <c r="H773" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I773" s="31"/>
     </row>
@@ -29373,7 +29371,7 @@
         <v>15</v>
       </c>
       <c r="H774" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I774" s="31"/>
     </row>
@@ -29398,7 +29396,7 @@
         <v>15</v>
       </c>
       <c r="H775" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I775" s="31"/>
     </row>
@@ -29423,7 +29421,7 @@
         <v>15</v>
       </c>
       <c r="H776" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I776" s="31"/>
     </row>
@@ -30150,7 +30148,7 @@
         <v>15</v>
       </c>
       <c r="H805" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I805" s="31"/>
     </row>
@@ -30175,7 +30173,7 @@
         <v>15</v>
       </c>
       <c r="H806" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I806" s="31"/>
     </row>
@@ -30200,7 +30198,7 @@
         <v>15</v>
       </c>
       <c r="H807" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I807" s="31"/>
     </row>
@@ -30225,7 +30223,7 @@
         <v>15</v>
       </c>
       <c r="H808" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I808" s="31"/>
     </row>
@@ -30250,7 +30248,7 @@
         <v>15</v>
       </c>
       <c r="H809" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I809" s="31"/>
     </row>
@@ -31406,7 +31404,7 @@
         <v>15</v>
       </c>
       <c r="H855" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I855" s="31"/>
     </row>
@@ -31431,7 +31429,7 @@
         <v>15</v>
       </c>
       <c r="H856" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I856" s="31"/>
     </row>
@@ -31456,7 +31454,7 @@
         <v>15</v>
       </c>
       <c r="H857" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I857" s="31"/>
     </row>
@@ -31481,7 +31479,7 @@
         <v>15</v>
       </c>
       <c r="H858" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I858" s="31"/>
     </row>
@@ -31506,7 +31504,7 @@
         <v>15</v>
       </c>
       <c r="H859" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I859" s="31"/>
     </row>
@@ -32212,7 +32210,7 @@
         <v>15</v>
       </c>
       <c r="H887" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I887" s="31"/>
     </row>
@@ -32237,7 +32235,7 @@
         <v>15</v>
       </c>
       <c r="H888" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I888" s="31"/>
     </row>
@@ -32262,7 +32260,7 @@
         <v>15</v>
       </c>
       <c r="H889" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I889" s="31"/>
     </row>
@@ -32287,7 +32285,7 @@
         <v>15</v>
       </c>
       <c r="H890" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I890" s="31"/>
     </row>
@@ -32312,7 +32310,7 @@
         <v>15</v>
       </c>
       <c r="H891" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I891" s="31"/>
     </row>
@@ -33589,7 +33587,7 @@
         <v>15</v>
       </c>
       <c r="H942" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I942" s="31"/>
     </row>
@@ -33614,7 +33612,7 @@
         <v>15</v>
       </c>
       <c r="H943" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I943" s="31"/>
     </row>
@@ -33639,7 +33637,7 @@
         <v>15</v>
       </c>
       <c r="H944" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I944" s="31"/>
     </row>
@@ -33664,7 +33662,7 @@
         <v>15</v>
       </c>
       <c r="H945" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I945" s="31"/>
     </row>
@@ -33689,7 +33687,7 @@
         <v>15</v>
       </c>
       <c r="H946" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I946" s="31"/>
     </row>
@@ -34716,7 +34714,7 @@
         <v>15</v>
       </c>
       <c r="H987" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I987" s="31"/>
     </row>
@@ -34741,7 +34739,7 @@
         <v>15</v>
       </c>
       <c r="H988" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I988" s="31"/>
     </row>
@@ -34766,7 +34764,7 @@
         <v>15</v>
       </c>
       <c r="H989" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I989" s="31"/>
     </row>
@@ -34791,7 +34789,7 @@
         <v>15</v>
       </c>
       <c r="H990" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I990" s="31"/>
     </row>
@@ -34816,7 +34814,7 @@
         <v>15</v>
       </c>
       <c r="H991" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I991" s="31"/>
     </row>
@@ -36093,7 +36091,7 @@
         <v>15</v>
       </c>
       <c r="H1042" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1042" s="31"/>
     </row>
@@ -36118,7 +36116,7 @@
         <v>15</v>
       </c>
       <c r="H1043" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1043" s="31"/>
     </row>
@@ -36143,7 +36141,7 @@
         <v>15</v>
       </c>
       <c r="H1044" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1044" s="31"/>
     </row>
@@ -36168,7 +36166,7 @@
         <v>15</v>
       </c>
       <c r="H1045" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1045" s="31"/>
     </row>
@@ -36193,7 +36191,7 @@
         <v>15</v>
       </c>
       <c r="H1046" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1046" s="31"/>
     </row>
@@ -37045,7 +37043,7 @@
         <v>15</v>
       </c>
       <c r="H1080" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1080" s="31"/>
     </row>
@@ -37070,7 +37068,7 @@
         <v>15</v>
       </c>
       <c r="H1081" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1081" s="31"/>
     </row>
@@ -37095,7 +37093,7 @@
         <v>15</v>
       </c>
       <c r="H1082" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1082" s="31"/>
     </row>
@@ -37120,7 +37118,7 @@
         <v>15</v>
       </c>
       <c r="H1083" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1083" s="31"/>
     </row>
@@ -37145,7 +37143,7 @@
         <v>15</v>
       </c>
       <c r="H1084" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1084" s="31"/>
     </row>
@@ -37697,7 +37695,7 @@
         <v>15</v>
       </c>
       <c r="H1106" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1106" s="31"/>
     </row>
@@ -37722,7 +37720,7 @@
         <v>15</v>
       </c>
       <c r="H1107" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1107" s="31"/>
     </row>
@@ -37747,7 +37745,7 @@
         <v>15</v>
       </c>
       <c r="H1108" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1108" s="31"/>
     </row>
@@ -37772,7 +37770,7 @@
         <v>15</v>
       </c>
       <c r="H1109" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1109" s="31"/>
     </row>
@@ -37797,7 +37795,7 @@
         <v>15</v>
       </c>
       <c r="H1110" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1110" s="31"/>
     </row>
@@ -38374,7 +38372,7 @@
         <v>15</v>
       </c>
       <c r="H1133" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1133" s="31"/>
     </row>
@@ -38399,7 +38397,7 @@
         <v>15</v>
       </c>
       <c r="H1134" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1134" s="31"/>
     </row>
@@ -38424,7 +38422,7 @@
         <v>15</v>
       </c>
       <c r="H1135" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1135" s="31"/>
     </row>
@@ -38449,7 +38447,7 @@
         <v>15</v>
       </c>
       <c r="H1136" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1136" s="31"/>
     </row>
@@ -38474,7 +38472,7 @@
         <v>15</v>
       </c>
       <c r="H1137" s="29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1137" s="31"/>
     </row>
@@ -42902,11 +42900,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42914,6 +42907,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I124 A1306:I1313 A1305:H1305 A20:H1302 A69:I1304">
@@ -42970,7 +42968,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C3 B19:B25 B78:B122 B125:B168 B171:B195 B201:B216 B229:B239 B241 B243 B245 B251:B252 B254:B260 B272:B273 B275:B281 B283:B286 B300:B309 B321:B327 B335:B342 B329:B333 B344:B356 B362:B369 B373:B375 B377:B402 B404:B412 B420:B429 B431:B438 B449:B457 B475:B477 B486:B514 B523:B588 B595:B618 B625:B633 B660:B696 B703:B732 B739:B770 B777:B803 B810:B838 B860:B885 B892:B905 B911:B940 B947:B972 B992:B1025 B1305:B1315 B1047:B1078 B1085:B1104 B1111:B1131 B1281:B1290 B1301:B1304 B1138:B1234 B1239:B1254 B1256:B1257 B1259:B1264 B1270:B1274 B458:B469 B634:B653 B839:B853 B973:B985 B1026:B1040" numberStoredAsText="1"/>
+    <ignoredError sqref="C3 B19:B328 B334:B343 B329:B333 B344:B448 B449:B457 B474:B624 B625:B633 B659:B809 B810:B838 B859:B946 B947:B972 B991:B1025 B1305:B1315 B1046:B1137 B1280:B1300 B1301:B1304 B1138:B1279 B458:B473 B634:B658 B839:B858 B973:B990 B1026:B1045" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
[MS-OXCMAPIHTTP] fix workitem 711962: Update capture code for latest RS
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -9108,21 +9108,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9146,6 +9131,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10088,127 +10088,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10221,12 +10221,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10239,12 +10239,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10257,12 +10257,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10275,60 +10275,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -32604,13 +32604,13 @@
         <v>19</v>
       </c>
       <c r="F903" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G903" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H903" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I903" s="31"/>
     </row>
@@ -32679,13 +32679,13 @@
         <v>19</v>
       </c>
       <c r="F906" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G906" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H906" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I906" s="31"/>
     </row>
@@ -32729,13 +32729,13 @@
         <v>19</v>
       </c>
       <c r="F908" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G908" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H908" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I908" s="31"/>
     </row>
@@ -32754,13 +32754,13 @@
         <v>19</v>
       </c>
       <c r="F909" s="29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G909" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H909" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I909" s="31"/>
     </row>
@@ -40999,7 +40999,7 @@
         <v>15</v>
       </c>
       <c r="H1238" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1238" s="31"/>
     </row>
@@ -42028,7 +42028,7 @@
         <v>15</v>
       </c>
       <c r="H1279" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1279" s="31"/>
     </row>
@@ -42900,6 +42900,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -42907,11 +42912,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I124 A1306:I1313 A1305:H1305 A20:H1302 A69:I1304">

</xml_diff>

<commit_message>
[MS-OXCMAPIHTTP] fix watchman error
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -8823,9 +8823,6 @@
     <t>MS-OXCMAPIHTTP_R2239</t>
   </si>
   <si>
-    <t>Verified by requirement: MS-OXCMAPIHTTP_R2237.</t>
-  </si>
-  <si>
     <t>MS-OXCMAPIHTTP_R590:i</t>
   </si>
   <si>
@@ -8911,6 +8908,9 @@
   </si>
   <si>
     <t>MS-OXCMAPIHTTP_R2004:c</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXCMAPIHTTP_R2237.</t>
   </si>
 </sst>
 </file>
@@ -9183,21 +9183,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9222,55 +9207,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <b val="0"/>
@@ -9609,6 +9565,80 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -9738,34 +9768,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1325" tableType="xml" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1325" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I1325"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="24">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="23">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="22">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="21">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="20">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="19">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="18">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="17">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="16">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -9774,12 +9804,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="10"/>
-    <tableColumn id="2" name="Test" dataDxfId="9"/>
-    <tableColumn id="3" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10163,127 +10193,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -10296,12 +10326,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -10314,12 +10344,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -10332,12 +10362,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -10350,60 +10380,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -10714,16 +10744,16 @@
     </row>
     <row r="31" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A31" s="22" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E31" s="22" t="s">
         <v>19</v>
@@ -10741,16 +10771,16 @@
     </row>
     <row r="32" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A32" s="22" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>19</v>
@@ -10768,16 +10798,16 @@
     </row>
     <row r="33" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A33" s="22" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E33" s="22" t="s">
         <v>19</v>
@@ -10795,16 +10825,16 @@
     </row>
     <row r="34" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A34" s="22" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>19</v>
@@ -10822,16 +10852,16 @@
     </row>
     <row r="35" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A35" s="22" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E35" s="22" t="s">
         <v>19</v>
@@ -10849,16 +10879,16 @@
     </row>
     <row r="36" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A36" s="22" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E36" s="22" t="s">
         <v>19</v>
@@ -10876,16 +10906,16 @@
     </row>
     <row r="37" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A37" s="22" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>19</v>
@@ -10903,16 +10933,16 @@
     </row>
     <row r="38" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A38" s="22" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>19</v>
@@ -10930,16 +10960,16 @@
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A39" s="22" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>19</v>
@@ -10957,16 +10987,16 @@
     </row>
     <row r="40" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A40" s="22" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>19</v>
@@ -10984,16 +11014,16 @@
     </row>
     <row r="41" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A41" s="22" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E41" s="22" t="s">
         <v>19</v>
@@ -11011,16 +11041,16 @@
     </row>
     <row r="42" spans="1:9" s="23" customFormat="1" ht="45">
       <c r="A42" s="22" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>1099</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="E42" s="22" t="s">
         <v>19</v>
@@ -11619,7 +11649,7 @@
         <v>1871</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="22" t="s">
@@ -15608,7 +15638,7 @@
         <v>15</v>
       </c>
       <c r="H222" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I222" s="31"/>
     </row>
@@ -25990,7 +26020,7 @@
       </c>
       <c r="I636" s="31"/>
     </row>
-    <row r="637" spans="1:9" ht="30">
+    <row r="637" spans="1:9" ht="45">
       <c r="A637" s="29" t="s">
         <v>504</v>
       </c>
@@ -26013,8 +26043,8 @@
       <c r="H637" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I637" s="20" t="s">
-        <v>2846</v>
+      <c r="I637" s="31" t="s">
+        <v>2875</v>
       </c>
     </row>
     <row r="638" spans="1:9" ht="30">
@@ -33003,13 +33033,13 @@
         <v>19</v>
       </c>
       <c r="F915" s="29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G915" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H915" s="29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I915" s="31"/>
     </row>
@@ -43068,10 +43098,10 @@
         <v>1223</v>
       </c>
       <c r="C1317" s="20" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="D1317" s="22" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="E1317" s="22" t="s">
         <v>22</v>
@@ -43086,7 +43116,7 @@
         <v>20</v>
       </c>
       <c r="I1317" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="1318" spans="1:9" ht="30">
@@ -43299,6 +43329,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -43306,41 +43341,58 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I20:I136 A1318:I1325 A1317:H1317 A81:I1316 A20:H1314">
-    <cfRule type="expression" dxfId="7" priority="53">
+  <conditionalFormatting sqref="I20:I136 A1318:I1325 A1317:H1317 A81:I636 A638:I1316 A20:H1314">
+    <cfRule type="expression" dxfId="32" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="31" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="61">
+    <cfRule type="expression" dxfId="30" priority="67">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I136 A1318:I1325 A1317:H1317 A81:I1316 A20:H1314">
-    <cfRule type="expression" dxfId="4" priority="7">
+  <conditionalFormatting sqref="I20:I136 A1318:I1325 A1317:H1317 A81:I636 A638:I1316 A20:H1314">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="28" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="27" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1325">
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="26" priority="19">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I637">
+    <cfRule type="expression" dxfId="24" priority="4">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="5">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="6">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I637">
+    <cfRule type="expression" dxfId="21" priority="1">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="2">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="3">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -43367,7 +43419,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C3 B43:B1327 B19:B30" numberStoredAsText="1"/>
+    <ignoredError sqref="C3 B42:B1327 B19:B41" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Update for MAPI package testing on E2016
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCMAPIHTTP/MS-OXCMAPIHTTP_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526E8EA7-1D1E-4134-8639-C2EE15945663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429F8AC5-B39D-4E85-9DA0-B88DE69E580E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9224,21 +9224,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9262,6 +9247,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10180,8 +10180,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10231,132 +10231,132 @@
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>43305</v>
+        <v>43445</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10369,12 +10369,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10387,12 +10387,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -10405,12 +10405,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10423,60 +10423,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="41" t="s">
         <v>2862</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -43382,6 +43382,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -43389,11 +43394,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I136 A1318:I1325 A81:I636 A638:I1314 A20:H1312 A1315:H1317">

</xml_diff>